<commit_message>
updated input output files
</commit_message>
<xml_diff>
--- a/Iron_speciation_calculator_input.xlsx
+++ b/Iron_speciation_calculator_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0149514\Documents\PhD\Coding\Feldspars and feldspathoids\Fe calc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0149514\Documents\PhD\Coding\Feldspars and feldspathoids\Fe_speciation_calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD0F17C-CD3B-4937-8389-21F47B8F75CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2099637-FB37-4260-B371-13C0BA4E602E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-13100" windowWidth="38620" windowHeight="21220" xr2:uid="{1D93F564-38D9-4AB4-9D6B-17D4FEB99DAF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1D93F564-38D9-4AB4-9D6B-17D4FEB99DAF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>sample_index</t>
   </si>
@@ -113,38 +113,32 @@
     <t>NiO_std</t>
   </si>
   <si>
-    <t>NM20ON179-NAB117</t>
-  </si>
-  <si>
     <t>MgO</t>
   </si>
   <si>
     <t>MgO_std</t>
   </si>
   <si>
-    <t>NY17-209-NAB117</t>
-  </si>
-  <si>
-    <t>AZKS052-NAB117</t>
-  </si>
-  <si>
-    <t>FOGO16-NAB117</t>
-  </si>
-  <si>
-    <t>TDC69-NAB117</t>
-  </si>
-  <si>
-    <t>NM20ON179-test_0</t>
-  </si>
-  <si>
     <t>pressure</t>
+  </si>
+  <si>
+    <t>02As1</t>
+  </si>
+  <si>
+    <t>01As1</t>
+  </si>
+  <si>
+    <t>12As1</t>
+  </si>
+  <si>
+    <t>07As1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +154,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -169,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -230,29 +245,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{8436E0FD-5625-4073-B020-F207E0A3BAF4}"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left/>
+        <right style="thin">
           <color indexed="64"/>
-        </left>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -278,19 +326,9 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
+        <left style="thin">
           <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
+        </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -346,105 +384,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>35</xdr:col>
-      <xdr:colOff>431800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D03C48D-B6D7-BE6F-D3A9-36F8803C5583}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="17348200" y="1016000"/>
-          <a:ext cx="3479800" cy="4254500"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100"/>
-            <a:t>Sample</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> index: Name of sample/identifying label</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>Temperature: Celcius</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t>Pressure:Pa</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4EC02A77-9072-4B6C-B794-ED8BCED2EB69}" name="Table1" displayName="Table1" ref="A1:AB1048576" totalsRowShown="0" headerRowBorderDxfId="6" headerRowCellStyle="Heading 3">
   <autoFilter ref="A1:AB1048576" xr:uid="{4EC02A77-9072-4B6C-B794-ED8BCED2EB69}"/>
   <tableColumns count="28">
     <tableColumn id="1" xr3:uid="{DF5E2169-535B-4311-8942-C98ADB477955}" name="sample_index" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{039EA453-2D9C-4D7C-8874-CD00A12A3CF2}" name="temperature" dataDxfId="4"/>
-    <tableColumn id="28" xr3:uid="{FE5B6271-6912-4C85-8FAC-5FDF0BED2301}" name="pressure" dataDxfId="0"/>
-    <tableColumn id="3" xr3:uid="{89880F7C-9807-4FFF-B34B-F6896C21E47A}" name="log_fO2" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{FE5B6271-6912-4C85-8FAC-5FDF0BED2301}" name="pressure" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{89880F7C-9807-4FFF-B34B-F6896C21E47A}" name="log_fO2" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{9CB00832-B95B-42E1-B458-1F3F80D32865}" name="SiO2"/>
     <tableColumn id="5" xr3:uid="{AC4F1451-E5C3-4824-A629-E2CA795B54EF}" name="TiO2"/>
     <tableColumn id="6" xr3:uid="{F760FBE8-7172-45AB-86E7-33553EFEA731}" name="Al2O3"/>
@@ -456,7 +403,7 @@
     <tableColumn id="12" xr3:uid="{07937F07-13F4-4122-AEB9-EB51C1D9656B}" name="K2O"/>
     <tableColumn id="13" xr3:uid="{94B4D900-0892-4EE4-8E83-AB875BDEFE95}" name="P2O5"/>
     <tableColumn id="14" xr3:uid="{C4F664B3-3DC5-46C2-8422-6D8B9CCDA9A1}" name="NiO"/>
-    <tableColumn id="15" xr3:uid="{3D1EA597-5511-4B69-8F22-FD0B833E1123}" name="Cr2O3" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{3D1EA597-5511-4B69-8F22-FD0B833E1123}" name="Cr2O3" dataDxfId="1"/>
     <tableColumn id="16" xr3:uid="{B9BB2D40-0934-4A67-9362-7D452A576DC2}" name="SiO2_std"/>
     <tableColumn id="17" xr3:uid="{89B90129-1505-47CA-91F2-B3EE3B8AE868}" name="TiO2_std"/>
     <tableColumn id="18" xr3:uid="{AE4A8DF7-811D-42D4-82AF-6C5DD7C7A1DF}" name="Al2O3_std"/>
@@ -468,7 +415,7 @@
     <tableColumn id="24" xr3:uid="{F02785E3-C74A-414B-9581-F970C8E6B766}" name="K2O_std"/>
     <tableColumn id="25" xr3:uid="{A4D9059C-AFA3-4CC0-8154-9B4F6BE2E69E}" name="P2O5_std"/>
     <tableColumn id="26" xr3:uid="{AFDA9CFF-118E-49A1-AAB0-1B2453FF84E8}" name="NiO_std"/>
-    <tableColumn id="27" xr3:uid="{6196E8CC-DFF5-46DA-B6D9-8D1494DE220A}" name="Cr2O3_std" dataDxfId="2"/>
+    <tableColumn id="27" xr3:uid="{6196E8CC-DFF5-46DA-B6D9-8D1494DE220A}" name="Cr2O3_std" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -774,13 +721,14 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V21" sqref="V21"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.21875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.77734375" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="13.77734375" style="5" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" style="5" customWidth="1"/>
     <col min="16" max="16" width="8.88671875" style="3"/>
     <col min="17" max="17" width="10.33203125" customWidth="1"/>
@@ -805,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>13</v>
@@ -826,7 +774,7 @@
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
@@ -862,7 +810,7 @@
         <v>18</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>19</v>
@@ -884,518 +832,334 @@
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1170</v>
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7">
+        <v>1593.15</v>
       </c>
       <c r="C2" s="5">
         <v>100000</v>
       </c>
       <c r="D2" s="5">
-        <v>-5.77</v>
+        <v>-7.09</v>
       </c>
       <c r="E2">
-        <v>46.247721819476887</v>
+        <v>46.66</v>
       </c>
       <c r="F2">
-        <v>3.248234780033938</v>
+        <v>2.4300000000000002</v>
       </c>
       <c r="G2">
-        <v>13.47279809674804</v>
+        <v>10.16</v>
       </c>
       <c r="H2">
-        <v>10.40723537655931</v>
+        <v>13.06</v>
       </c>
       <c r="I2">
-        <v>0.17715312150705451</v>
+        <v>0.19</v>
       </c>
       <c r="J2">
-        <v>7.8888058642526362</v>
+        <v>13.15</v>
       </c>
       <c r="K2">
-        <v>13.254934407861461</v>
+        <v>11.64</v>
       </c>
       <c r="L2">
-        <v>2.4315816149720511</v>
+        <v>1.95</v>
       </c>
       <c r="M2">
-        <v>2.3156924535866898</v>
+        <v>0.49</v>
       </c>
       <c r="N2">
-        <v>0.52733537132116381</v>
-      </c>
-      <c r="O2">
-        <v>1.257957421043516E-2</v>
+        <v>0.17</v>
       </c>
       <c r="P2" s="3">
-        <v>1.5927519470323021E-2</v>
+        <v>0.13</v>
       </c>
       <c r="Q2">
-        <v>0.1501304254816227</v>
+        <v>0.35</v>
       </c>
       <c r="R2">
-        <v>5.4780402088370372E-2</v>
+        <v>0.17</v>
       </c>
       <c r="S2">
-        <v>8.2397069421951144E-2</v>
+        <v>0.1</v>
       </c>
       <c r="T2">
-        <v>0.28331743875163329</v>
+        <v>0.22</v>
       </c>
       <c r="U2">
-        <v>2.4013306697784891E-2</v>
+        <v>0.34</v>
       </c>
       <c r="V2">
-        <v>6.6345666769409437E-2</v>
+        <v>0.1</v>
       </c>
       <c r="W2">
-        <v>0.19497493448700129</v>
+        <v>0.26</v>
       </c>
       <c r="X2">
-        <v>2.4843151509908509E-2</v>
+        <v>0.2</v>
       </c>
       <c r="Y2">
-        <v>4.4814062226521303E-2</v>
+        <v>0.04</v>
       </c>
       <c r="Z2">
-        <v>5.4433169152551447E-2</v>
-      </c>
-      <c r="AA2">
-        <v>3.03299873384557E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AB2" s="3">
-        <v>2.211671603802938E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" s="5">
-        <v>1170</v>
+      <c r="A3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1575.15</v>
       </c>
       <c r="C3" s="5">
         <v>100000</v>
       </c>
       <c r="D3" s="5">
-        <v>-5.77</v>
+        <v>-7.28</v>
       </c>
       <c r="E3">
-        <v>41.935407648286372</v>
+        <v>46.96</v>
       </c>
       <c r="F3">
-        <v>3.6558502144629812</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="G3">
-        <v>12.24160520132706</v>
+        <v>10.34</v>
       </c>
       <c r="H3">
-        <v>10.97792987023529</v>
+        <v>13.21</v>
       </c>
       <c r="I3">
-        <v>0.20785253100376211</v>
+        <v>0.2</v>
       </c>
       <c r="J3">
-        <v>8.4426072645236943</v>
+        <v>12.16</v>
       </c>
       <c r="K3">
-        <v>16.701452998140098</v>
+        <v>11.81</v>
       </c>
       <c r="L3">
-        <v>2.5341029530315158</v>
+        <v>1.84</v>
       </c>
       <c r="M3">
-        <v>2.21016273549882</v>
+        <v>0.44</v>
       </c>
       <c r="N3">
-        <v>1.0328192172291091</v>
-      </c>
-      <c r="O3">
-        <v>3.4282028858195361E-2</v>
+        <v>0.2</v>
       </c>
       <c r="P3" s="3">
-        <v>2.5927337403101991E-2</v>
+        <v>0.13</v>
       </c>
       <c r="Q3">
-        <v>0.25257018894824929</v>
+        <v>0.48</v>
       </c>
       <c r="R3">
-        <v>0.1831452543953116</v>
+        <v>0.11</v>
       </c>
       <c r="S3">
-        <v>8.9664487494259454E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T3">
-        <v>0.46733735574154872</v>
+        <v>0.2</v>
       </c>
       <c r="U3">
-        <v>1.9052058369947809E-2</v>
+        <v>0.21</v>
       </c>
       <c r="V3">
-        <v>0.26502512642138049</v>
+        <v>0.1</v>
       </c>
       <c r="W3">
-        <v>0.33664303571614718</v>
+        <v>0.12</v>
       </c>
       <c r="X3">
-        <v>0.11449318702102559</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="Y3">
-        <v>2.7429823829524011E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Z3">
-        <v>8.7918290147900147E-2</v>
-      </c>
-      <c r="AA3">
-        <v>4.3071305655973939E-2</v>
+        <v>0.03</v>
       </c>
       <c r="AB3" s="3">
-        <v>2.9903138592216209E-2</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>29</v>
+      <c r="A4" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="B4" s="5">
-        <v>1170</v>
+        <v>1593.15</v>
       </c>
       <c r="C4" s="5">
         <v>100000</v>
       </c>
       <c r="D4" s="5">
-        <v>-5.77</v>
+        <v>-5.09</v>
       </c>
       <c r="E4">
-        <v>47.535734992928361</v>
+        <v>46.36</v>
       </c>
       <c r="F4">
-        <v>2.970343745918866</v>
+        <v>2.4</v>
       </c>
       <c r="G4">
-        <v>14.685915552930449</v>
+        <v>10.07</v>
       </c>
       <c r="H4">
-        <v>10.28885856812315</v>
+        <v>12.34</v>
       </c>
       <c r="I4">
-        <v>0.14857456302802491</v>
+        <v>0.2</v>
       </c>
       <c r="J4">
-        <v>8.453016148752182</v>
+        <v>13.87</v>
       </c>
       <c r="K4">
-        <v>12.274053762452249</v>
+        <v>11.48</v>
       </c>
       <c r="L4">
-        <v>2.4691761021352772</v>
+        <v>1.95</v>
       </c>
       <c r="M4">
-        <v>0.6147024639909322</v>
+        <v>0.46</v>
       </c>
       <c r="N4">
-        <v>0.52240411070008697</v>
-      </c>
-      <c r="O4">
-        <v>2.5028865180673342E-2</v>
+        <v>0.21</v>
       </c>
       <c r="P4" s="3">
-        <v>1.219112385974188E-2</v>
+        <v>0.13</v>
       </c>
       <c r="Q4">
-        <v>0.1754662341382737</v>
+        <v>0.39</v>
       </c>
       <c r="R4">
-        <v>0.14727613276364129</v>
+        <v>0.1</v>
       </c>
       <c r="S4">
-        <v>0.1244536243441082</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="T4">
-        <v>0.29616166551951317</v>
+        <v>0.22</v>
       </c>
       <c r="U4">
-        <v>3.2289902068180741E-2</v>
+        <v>0.35</v>
       </c>
       <c r="V4">
-        <v>9.8747547845526334E-2</v>
+        <v>0.09</v>
       </c>
       <c r="W4">
-        <v>0.1565975795742735</v>
+        <v>0.26</v>
       </c>
       <c r="X4">
-        <v>0.15580868879292209</v>
+        <v>0.21</v>
       </c>
       <c r="Y4">
-        <v>4.0070368565349429E-2</v>
+        <v>0.06</v>
       </c>
       <c r="Z4">
-        <v>4.8395163412707012E-2</v>
-      </c>
-      <c r="AA4">
-        <v>3.1296655916348462E-2</v>
+        <v>0.04</v>
       </c>
       <c r="AB4" s="3">
-        <v>1.8810196795701589E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>30</v>
+      <c r="A5" s="9" t="s">
+        <v>31</v>
       </c>
       <c r="B5" s="5">
-        <v>1170</v>
+        <v>1575.15</v>
       </c>
       <c r="C5" s="5">
         <v>100000</v>
       </c>
       <c r="D5" s="5">
-        <v>-5.77</v>
+        <v>-5.28</v>
       </c>
       <c r="E5">
-        <v>44.769360028983407</v>
+        <v>46.83</v>
       </c>
       <c r="F5">
-        <v>3.274604616823265</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="G5">
-        <v>13.55417845409284</v>
+        <v>10.39</v>
       </c>
       <c r="H5">
-        <v>11.39663279467389</v>
+        <v>12.72</v>
       </c>
       <c r="I5">
-        <v>0.20381611424619489</v>
+        <v>0.2</v>
       </c>
       <c r="J5">
-        <v>8.4728141138016095</v>
+        <v>12.61</v>
       </c>
       <c r="K5">
-        <v>14.43763722855619</v>
+        <v>11.72</v>
       </c>
       <c r="L5">
-        <v>1.8844077242542201</v>
+        <v>1.99</v>
       </c>
       <c r="M5">
-        <v>1.100563934503247</v>
+        <v>0.48</v>
       </c>
       <c r="N5">
-        <v>0.86017340147798294</v>
-      </c>
-      <c r="O5">
-        <v>2.954306032107859E-2</v>
+        <v>0.21</v>
       </c>
       <c r="P5" s="3">
-        <v>1.6268528266074798E-2</v>
+        <v>0.12</v>
       </c>
       <c r="Q5">
-        <v>0.35168641092438607</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="R5">
-        <v>0.21032730886850551</v>
+        <v>0.19</v>
       </c>
       <c r="S5">
-        <v>0.1094992923305622</v>
+        <v>0.1</v>
       </c>
       <c r="T5">
-        <v>0.27337861452663248</v>
+        <v>0.13</v>
       </c>
       <c r="U5">
-        <v>4.7058058425361912E-2</v>
+        <v>0.3</v>
       </c>
       <c r="V5">
-        <v>9.0525415275828858E-2</v>
+        <v>0.1</v>
       </c>
       <c r="W5">
-        <v>0.17401609288584899</v>
+        <v>0.22</v>
       </c>
       <c r="X5">
-        <v>0.1219500156166438</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="Y5">
-        <v>4.1231880078298797E-2</v>
+        <v>0.05</v>
       </c>
       <c r="Z5">
-        <v>4.4732423794144348E-2</v>
-      </c>
-      <c r="AA5">
-        <v>3.6494354231071557E-2</v>
+        <v>0.05</v>
       </c>
       <c r="AB5" s="3">
-        <v>1.5852425827897001E-2</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1170</v>
-      </c>
-      <c r="C6" s="5">
-        <v>100000</v>
-      </c>
-      <c r="D6" s="5">
-        <v>-5.77</v>
-      </c>
-      <c r="E6">
-        <v>45.970172698586772</v>
-      </c>
-      <c r="F6">
-        <v>3.371517877675565</v>
-      </c>
-      <c r="G6">
-        <v>13.13718570157104</v>
-      </c>
-      <c r="H6">
-        <v>11.817336534403321</v>
-      </c>
-      <c r="I6">
-        <v>0.1581924553554743</v>
-      </c>
-      <c r="J6">
-        <v>7.8841443273043854</v>
-      </c>
-      <c r="K6">
-        <v>13.06600880894915</v>
-      </c>
-      <c r="L6">
-        <v>2.3687052949931151</v>
-      </c>
-      <c r="M6">
-        <v>1.6923704933143009</v>
-      </c>
-      <c r="N6">
-        <v>0.50337157912711739</v>
-      </c>
-      <c r="O6">
-        <v>1.3264559052794391E-2</v>
-      </c>
-      <c r="P6" s="3">
-        <v>1.7729669666959231E-2</v>
-      </c>
-      <c r="Q6">
-        <v>0.24723119592410109</v>
-      </c>
-      <c r="R6">
-        <v>0.15287811006807769</v>
-      </c>
-      <c r="S6">
-        <v>0.1305099029968298</v>
-      </c>
-      <c r="T6">
-        <v>0.40183386988943109</v>
-      </c>
-      <c r="U6">
-        <v>3.1720439457866047E-2</v>
-      </c>
-      <c r="V6">
-        <v>7.7891495466919147E-2</v>
-      </c>
-      <c r="W6">
-        <v>0.1268568049800641</v>
-      </c>
-      <c r="X6">
-        <v>9.1133901063127423E-2</v>
-      </c>
-      <c r="Y6">
-        <v>2.5368999145985949E-2</v>
-      </c>
-      <c r="Z6">
-        <v>6.9085622470192842E-2</v>
-      </c>
-      <c r="AA6">
-        <v>1.78118889659401E-2</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>2.1225411954031829E-2</v>
-      </c>
+      <c r="A6"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="5">
-        <v>1170</v>
-      </c>
-      <c r="C7" s="5">
-        <v>100000</v>
-      </c>
-      <c r="D7" s="5">
-        <v>-5.77</v>
-      </c>
-      <c r="E7">
-        <v>46.247721819476887</v>
-      </c>
-      <c r="F7">
-        <v>3.248234780033938</v>
-      </c>
-      <c r="G7">
-        <v>13.47279809674804</v>
-      </c>
-      <c r="H7">
-        <v>10.40723537655931</v>
-      </c>
-      <c r="I7">
-        <v>0.17715312150705451</v>
-      </c>
-      <c r="J7">
-        <v>7.8888058642526362</v>
-      </c>
-      <c r="K7">
-        <v>13.254934407861461</v>
-      </c>
-      <c r="L7">
-        <v>2.4315816149720511</v>
-      </c>
-      <c r="M7">
-        <v>2.3156924535866898</v>
-      </c>
-      <c r="N7">
-        <v>0.52733537132116381</v>
-      </c>
-      <c r="P7" s="3">
-        <v>1.5927519470323021E-2</v>
-      </c>
-      <c r="Q7">
-        <v>0.1501304254816227</v>
-      </c>
-      <c r="R7">
-        <v>5.4780402088370372E-2</v>
-      </c>
-      <c r="S7">
-        <v>8.2397069421951144E-2</v>
-      </c>
-      <c r="T7">
-        <v>0.28331743875163329</v>
-      </c>
-      <c r="U7">
-        <v>2.4013306697784891E-2</v>
-      </c>
-      <c r="V7">
-        <v>6.6345666769409437E-2</v>
-      </c>
-      <c r="W7">
-        <v>0.19497493448700129</v>
-      </c>
-      <c r="X7">
-        <v>2.4843151509908509E-2</v>
-      </c>
-      <c r="Y7">
-        <v>4.4814062226521303E-2</v>
-      </c>
-      <c r="Z7">
-        <v>5.4433169152551447E-2</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>2.211671603802938E-2</v>
-      </c>
+      <c r="A7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>

</xml_diff>